<commit_message>
Before recovering the float levers
</commit_message>
<xml_diff>
--- a/2_formulation/optimization_parameters.xlsx
+++ b/2_formulation/optimization_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\Documents\GitHub\GDL_Aquapheric_Policies\2_formulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E93DDECB-EDDB-4ED2-869F-AE1ADC8A0459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955C275F-6A95-4246-A285-600C989A5DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B24E5F51-ECD3-4BAD-BDA9-992338CB29CA}"/>
+    <workbookView xWindow="-20856" yWindow="-4692" windowWidth="17280" windowHeight="8880" xr2:uid="{B24E5F51-ECD3-4BAD-BDA9-992338CB29CA}"/>
   </bookViews>
   <sheets>
     <sheet name="optimization_parameters" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>experiment_name</t>
   </si>
@@ -98,12 +98,6 @@
   </si>
   <si>
     <t>Sup. Dem. Deficit, Energy &amp; Sup. PerCap. GINI</t>
-  </si>
-  <si>
-    <t>Sup. Dem. Deficit, Energy, Sup. PerCap. GINI  &amp; Sufficientarians</t>
-  </si>
-  <si>
-    <t>Average Sup. PerCap</t>
   </si>
   <si>
     <t>Supplied Demand Deficit</t>
@@ -984,27 +978,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22B6DB64-4E84-4F03-98BA-AF058EBF7997}">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
-    <col min="2" max="12" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="1" customWidth="1"/>
+    <col min="2" max="12" width="19.5703125" customWidth="1"/>
     <col min="13" max="15" width="7" customWidth="1"/>
-    <col min="17" max="17" width="16.5546875" customWidth="1"/>
-    <col min="18" max="18" width="17.109375" customWidth="1"/>
-    <col min="19" max="19" width="14.5546875" customWidth="1"/>
-    <col min="20" max="20" width="17.88671875" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1075,12 +1069,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="b">
         <v>0</v>
@@ -1095,7 +1089,7 @@
         <v>0</v>
       </c>
       <c r="G2" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2" t="b">
         <v>0</v>
@@ -1143,9 +1137,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1160,7 +1154,7 @@
         <v>0</v>
       </c>
       <c r="F3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
@@ -1178,7 +1172,7 @@
         <v>0</v>
       </c>
       <c r="L3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3">
         <v>10000</v>
@@ -1211,9 +1205,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1231,19 +1225,19 @@
         <v>1</v>
       </c>
       <c r="G4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L4" t="b">
         <v>1</v>
@@ -1279,168 +1273,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B5" t="b">
-        <v>1</v>
-      </c>
-      <c r="C5" t="b">
-        <v>0</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-      <c r="E5" t="b">
-        <v>0</v>
-      </c>
-      <c r="F5" t="b">
-        <v>1</v>
-      </c>
-      <c r="G5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H5" t="b">
-        <v>1</v>
-      </c>
-      <c r="I5" t="b">
-        <v>0</v>
-      </c>
-      <c r="J5" t="b">
-        <v>1</v>
-      </c>
-      <c r="K5" t="b">
-        <v>1</v>
-      </c>
-      <c r="L5" t="b">
-        <v>1</v>
-      </c>
-      <c r="M5">
-        <v>10000</v>
-      </c>
-      <c r="N5">
-        <v>0.01</v>
-      </c>
-      <c r="O5">
-        <v>1</v>
-      </c>
-      <c r="P5" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-      <c r="R5">
-        <v>1</v>
-      </c>
-      <c r="S5">
-        <v>1</v>
-      </c>
-      <c r="T5">
-        <v>1</v>
-      </c>
-      <c r="U5" t="b">
-        <v>1</v>
-      </c>
-      <c r="V5" t="s">
-        <v>2</v>
-      </c>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B6" t="b">
-        <v>1</v>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
-      <c r="F6" t="b">
-        <v>1</v>
-      </c>
-      <c r="G6" t="b">
-        <v>1</v>
-      </c>
-      <c r="H6" t="b">
-        <v>1</v>
-      </c>
-      <c r="I6" t="b">
-        <v>0</v>
-      </c>
-      <c r="J6" t="b">
-        <v>1</v>
-      </c>
-      <c r="K6" t="b">
-        <v>1</v>
-      </c>
-      <c r="L6" t="b">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>10000</v>
-      </c>
-      <c r="N6">
-        <v>0.01</v>
-      </c>
-      <c r="O6">
-        <v>1</v>
-      </c>
-      <c r="P6" t="s">
-        <v>7</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-      <c r="R6">
-        <v>1</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6" t="b">
-        <v>1</v>
-      </c>
-      <c r="V6" t="s">
-        <v>2</v>
-      </c>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:L19">
+  <conditionalFormatting sqref="B2:L17">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TRUE">
       <formula>NOT(ISERROR(SEARCH("TRUE",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:L19" xr:uid="{20655019-481A-4CDF-8344-41D61E25604F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:L17" xr:uid="{20655019-481A-4CDF-8344-41D61E25604F}">
       <formula1>"True, False"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1450,6 +1308,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F145FA38EFD6D645960FBC0DDB903B21" ma:contentTypeVersion="11" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="f41eb4abd417e8724364d9841165d35a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="cd5db80a-28fe-45ff-85db-1519f069e397" xmlns:ns4="e015ac9b-3df2-44de-9ba6-1f54a1c2d7fa" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0fc0f3ee15e4e52d88faf4e9004b5dea" ns3:_="" ns4:_="">
     <xsd:import namespace="cd5db80a-28fe-45ff-85db-1519f069e397"/>
@@ -1656,15 +1523,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -1674,6 +1532,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89F5CE74-5B4F-4E70-BB1C-EE845C2C0DD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6180361C-C4E4-45B9-B0ED-223A1A269A35}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1688,14 +1554,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89F5CE74-5B4F-4E70-BB1C-EE845C2C0DD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Everything working for app deployment
</commit_message>
<xml_diff>
--- a/2_formulation/optimization_parameters.xlsx
+++ b/2_formulation/optimization_parameters.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\Documents\GitHub\GDL_Aquapheric_Policies\2_formulation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\Documents\GitHub\GDL_Aquapheric_Policies - Copy\2_formulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{955C275F-6A95-4246-A285-600C989A5DFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FB12FB8-BDA4-4A75-8344-D76300AFC794}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20856" yWindow="-4692" windowWidth="17280" windowHeight="8880" xr2:uid="{B24E5F51-ECD3-4BAD-BDA9-992338CB29CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B24E5F51-ECD3-4BAD-BDA9-992338CB29CA}"/>
   </bookViews>
   <sheets>
     <sheet name="optimization_parameters" sheetId="2" r:id="rId1"/>
@@ -981,10 +981,10 @@
   <dimension ref="A1:W10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F6" sqref="F6"/>
+      <selection pane="bottomRight" activeCell="F4" sqref="E4:F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1219,7 +1219,7 @@
         <v>0</v>
       </c>
       <c r="E4" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
@@ -1228,16 +1228,16 @@
         <v>1</v>
       </c>
       <c r="H4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I4" t="b">
         <v>0</v>
       </c>
       <c r="J4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L4" t="b">
         <v>1</v>
@@ -1308,12 +1308,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cd5db80a-28fe-45ff-85db-1519f069e397" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1524,17 +1523,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cd5db80a-28fe-45ff-85db-1519f069e397" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89F5CE74-5B4F-4E70-BB1C-EE845C2C0DD5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33A84DA-5313-4F68-9E7D-8A3C941BC69A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="cd5db80a-28fe-45ff-85db-1519f069e397"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e015ac9b-3df2-44de-9ba6-1f54a1c2d7fa"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1559,18 +1568,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33A84DA-5313-4F68-9E7D-8A3C941BC69A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89F5CE74-5B4F-4E70-BB1C-EE845C2C0DD5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="cd5db80a-28fe-45ff-85db-1519f069e397"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e015ac9b-3df2-44de-9ba6-1f54a1c2d7fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changes to the compromise policy implementation and analysis
</commit_message>
<xml_diff>
--- a/2_formulation/optimization_parameters.xlsx
+++ b/2_formulation/optimization_parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ariel\Documents\GitHub\GoldinThesis-GDL_AqP\2_formulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FADEC0-B25C-461A-8F9E-A9D837A9BFDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE547A45-85C6-4C45-AC74-DEBFEBD64131}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B24E5F51-ECD3-4BAD-BDA9-992338CB29CA}"/>
+    <workbookView xWindow="3465" yWindow="3465" windowWidth="21600" windowHeight="11295" xr2:uid="{B24E5F51-ECD3-4BAD-BDA9-992338CB29CA}"/>
   </bookViews>
   <sheets>
     <sheet name="optimization_parameters" sheetId="2" r:id="rId1"/>
@@ -110,13 +110,13 @@
     <t>supply_percapita</t>
   </si>
   <si>
-    <t>Supplied Demand Deficit</t>
-  </si>
-  <si>
-    <t>Sup. Dem. Deficit, Energy &amp; All Justice</t>
-  </si>
-  <si>
-    <t>Sup. Dem. Deficit, Sup. Percap. GINI &amp; Energy</t>
+    <t>A-posteriori</t>
+  </si>
+  <si>
+    <t>Mixed</t>
+  </si>
+  <si>
+    <t>A-priori</t>
   </si>
 </sst>
 </file>
@@ -997,21 +997,21 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.33203125" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.6640625" style="1" customWidth="1"/>
-    <col min="2" max="12" width="19.5546875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="1" customWidth="1"/>
+    <col min="2" max="12" width="19.5703125" customWidth="1"/>
     <col min="13" max="15" width="7" customWidth="1"/>
-    <col min="17" max="17" width="16.5546875" customWidth="1"/>
-    <col min="18" max="18" width="17.109375" customWidth="1"/>
-    <col min="19" max="19" width="14.5546875" customWidth="1"/>
-    <col min="20" max="20" width="17.88671875" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" customWidth="1"/>
+    <col min="18" max="18" width="17.140625" customWidth="1"/>
+    <col min="19" max="19" width="14.5703125" customWidth="1"/>
+    <col min="20" max="20" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="1" customFormat="1" ht="47.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="1" customFormat="1" ht="47.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1082,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>25</v>
       </c>
@@ -1150,9 +1150,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B3" t="b">
         <v>1</v>
@@ -1218,9 +1218,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B4" t="b">
         <v>1</v>
@@ -1286,19 +1286,19 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2"/>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
     </row>
   </sheetData>
@@ -1318,12 +1318,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="cd5db80a-28fe-45ff-85db-1519f069e397" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1534,17 +1533,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="cd5db80a-28fe-45ff-85db-1519f069e397" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89F5CE74-5B4F-4E70-BB1C-EE845C2C0DD5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33A84DA-5313-4F68-9E7D-8A3C941BC69A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="cd5db80a-28fe-45ff-85db-1519f069e397"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="e015ac9b-3df2-44de-9ba6-1f54a1c2d7fa"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1569,18 +1578,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33A84DA-5313-4F68-9E7D-8A3C941BC69A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{89F5CE74-5B4F-4E70-BB1C-EE845C2C0DD5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="cd5db80a-28fe-45ff-85db-1519f069e397"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="e015ac9b-3df2-44de-9ba6-1f54a1c2d7fa"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>